<commit_message>
encrypt link and change register users
</commit_message>
<xml_diff>
--- a/uploads/excel/Prueba10.xlsx
+++ b/uploads/excel/Prueba10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLASSROOM-BACKEND\classroom-backend\uploads\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B82C8C0-D985-4258-8DE9-3D1923CA5F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6E2B8A-FF0B-4EFB-B16A-834D7F998346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="180" windowWidth="12180" windowHeight="13740" xr2:uid="{55A72A1F-5D96-40D5-8101-8FD384097781}"/>
+    <workbookView xWindow="5100" yWindow="720" windowWidth="19665" windowHeight="13740" xr2:uid="{55A72A1F-5D96-40D5-8101-8FD384097781}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>Nombres</t>
   </si>
@@ -54,40 +54,70 @@
     <t>Ciclo</t>
   </si>
   <si>
-    <t xml:space="preserve">Aquilino </t>
-  </si>
-  <si>
-    <t>Eloy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pascual </t>
-  </si>
-  <si>
-    <t>Pedro Miguel</t>
-  </si>
-  <si>
-    <t>Cristian Acev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Francisco Luis </t>
-  </si>
-  <si>
-    <t>Marti Cha</t>
-  </si>
-  <si>
-    <t>Luis Javier Pos</t>
-  </si>
-  <si>
-    <t>Ivan Sevil</t>
-  </si>
-  <si>
-    <t>Damian Mon</t>
-  </si>
-  <si>
-    <t>ANUAL</t>
-  </si>
-  <si>
-    <t>Matecero</t>
+    <t>Aquilino robert</t>
+  </si>
+  <si>
+    <t>Eloy ticona</t>
+  </si>
+  <si>
+    <t>Pascual  perez</t>
+  </si>
+  <si>
+    <t>Pedro Miguel  lopez</t>
+  </si>
+  <si>
+    <t>Cristian Acev tipo</t>
+  </si>
+  <si>
+    <t>Francisco Luis  juarez</t>
+  </si>
+  <si>
+    <t>Marti Cha  perez</t>
+  </si>
+  <si>
+    <t>Luis Javier Pos lipo</t>
+  </si>
+  <si>
+    <t>Ivan Sevil  tica</t>
+  </si>
+  <si>
+    <t>Damian Mon  morales</t>
+  </si>
+  <si>
+    <t>ab10</t>
+  </si>
+  <si>
+    <t>ab20</t>
+  </si>
+  <si>
+    <t>ab30</t>
+  </si>
+  <si>
+    <t>ab40</t>
+  </si>
+  <si>
+    <t>ab50</t>
+  </si>
+  <si>
+    <t>ab60</t>
+  </si>
+  <si>
+    <t>ab70</t>
+  </si>
+  <si>
+    <t>ab80</t>
+  </si>
+  <si>
+    <t>ab90</t>
+  </si>
+  <si>
+    <t>ab100</t>
+  </si>
+  <si>
+    <t>VERANO</t>
+  </si>
+  <si>
+    <t>Ciencias</t>
   </si>
 </sst>
 </file>
@@ -458,7 +488,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,13 +526,13 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>47416307</v>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E2">
         <v>47416308</v>
@@ -514,18 +544,18 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
-        <v>47616308</v>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E3">
         <v>47416308</v>
@@ -537,18 +567,18 @@
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>47216308</v>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E4">
         <v>47416308</v>
@@ -560,18 +590,18 @@
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>47412308</v>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E5">
         <v>47416308</v>
@@ -583,18 +613,18 @@
         <v>6</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>47416908</v>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E6">
         <v>47416308</v>
@@ -606,18 +636,18 @@
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
-        <v>47416300</v>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E7">
         <v>47416308</v>
@@ -629,18 +659,18 @@
         <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
-        <v>47516308</v>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E8">
         <v>47416308</v>
@@ -652,18 +682,18 @@
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9">
-        <v>47486308</v>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E9">
         <v>47416308</v>
@@ -675,18 +705,18 @@
         <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
-        <v>47417308</v>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E10">
         <v>47416308</v>
@@ -698,18 +728,18 @@
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
-        <v>47413308</v>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="E11">
         <v>47416308</v>
@@ -721,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>